<commit_message>
.amind, título com arquivo, Novo, Cores/Fonte em seleção, padrões, export PNG
</commit_message>
<xml_diff>
--- a/prompts.xlsx
+++ b/prompts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\Amarelo\Amarelo Mind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{1C4A51C3-FE6D-488F-A0E1-8A833BA1AADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF06ED1A-1710-4E74-8AC9-778D361CB6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8A4AF20B-E298-4B71-8849-2ED57E01A954}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="103">
   <si>
     <t>Objetivo</t>
   </si>
@@ -318,10 +317,34 @@
     <t>Deve adicionar um retângulo na tela, sem borda, com sombra lateral, background amarelo e pronto para receber texto (se o usuário adicionar um objeto e começar a digitar, o texto já deve ser inserido nos limites das margens da figura, de forma justificada. O texto pode quebrar linhas dentro da figura. Se um objeto já estiver selecionado quando o usuário teclar "+" ou clicar no botão Adicionar, o objeto selecionado será duplicado, preservando o background atual, sombra (se houver) e descartando o conteúdo do objeto.</t>
   </si>
   <si>
-    <t xml:space="preserve">Todos os botões devem ser quadrados, sem texto, sem borda, apenas com ícones. Uma legenda alt deve aparecer enquanto o o  ponteiro estiver sobre o botão. O ícones de todos os botões estão em assets\icons\ e o ícone do app é app_icon.png. </t>
-  </si>
-  <si>
     <t>O design do app deve parecer moderno e bonito, com luzes, degradês, sofisticação e profundidade.</t>
+  </si>
+  <si>
+    <t>problemas</t>
+  </si>
+  <si>
+    <t>um objeto já é adicionado com sombra, por padrão. O usuário pode tirar, se quiser, clicando no botão.</t>
+  </si>
+  <si>
+    <t>o usuário pode mover a tela de duas formas: ou pelas setas do teclado, se não houver nenhum objeto selecionado, ou pressionando  com o botão direito do mouse sobre um ponto vazio da tela e arrastando-o.</t>
+  </si>
+  <si>
+    <t>se um objeto estiver selecionado, as setas podem ser usadas para movê-lo, ou o ponteiro do mouse (clicando e arrastando)</t>
+  </si>
+  <si>
+    <t>o botão esquerdo do mouse ativa a seleção retangular, para selecionar objetos.</t>
+  </si>
+  <si>
+    <t>se um texto estiver selecionado, o botão cor deve estar habilitado, para alterar a cor desse texto.</t>
+  </si>
+  <si>
+    <t>as formatações de fonte não estao sendo aplicadas.</t>
+  </si>
+  <si>
+    <t>quando um objeto é excluído, as linhas conectadas a ele até então também devem ser, automaticamente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Todos os botões devem ser quadrados, sem texto, sem borda, apenas com ícones. Uma legenda alt deve aparecer enquanto o o  ponteiro estiver sobre o botão. O ícones de todos os botões estão em assets\icons\ e o ícone do app é App_icon.png. </t>
   </si>
 </sst>
 </file>
@@ -377,15 +400,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
@@ -411,6 +430,15 @@
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -747,892 +775,1021 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{762697AE-20C4-4A6F-A256-691AC23C2C91}">
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D91"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection sqref="A1:D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="22" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.140625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" style="4" customWidth="1"/>
     <col min="5" max="7" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="D2" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="C4" s="6" t="s">
+      <c r="D3" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="5" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="C8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="6" t="s">
+    <row r="8" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="5" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>3</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="5" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="6" t="s">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="5" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
         <v>4</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C17" s="5" t="s">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C17" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="C18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="6" t="s">
+    <row r="18" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="C18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="5" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>5</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="5" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="C23" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D23" s="6" t="s">
+    <row r="23" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="C23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="5" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>6</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="5" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C28" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="6" t="s">
+    <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C28" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="5" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
         <v>7</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="5" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C32" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C33" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="6" t="s">
+    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C33" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="5" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="7"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
         <v>8</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C37" s="5" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="D37" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="6" t="s">
+    <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C38" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5" t="s">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C39" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D39" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
         <v>9</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5" t="s">
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C42" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-    </row>
-    <row r="43" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="6" t="s">
+    </row>
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C43" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5" t="s">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-    </row>
-    <row r="45" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="10"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-    </row>
-    <row r="46" spans="1:7" s="3" customFormat="1" ht="195" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="7"/>
+    </row>
+    <row r="46" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
         <v>10</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C46" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D46" s="6" t="s">
+      <c r="C46" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-    </row>
-    <row r="47" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="10"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
-        <v>11</v>
-      </c>
-      <c r="B48" s="5" t="s">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>11</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D48" s="6" t="s">
+      <c r="D48" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C49" s="5" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C49" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D49" s="6" t="s">
+      <c r="D49" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="210" x14ac:dyDescent="0.25">
-      <c r="C50" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D50" s="6" t="s">
+    <row r="50" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+      <c r="C50" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C51" s="5" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C51" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D51" s="6" t="s">
+      <c r="D51" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="10"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="7"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
         <v>12</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D53" s="4" t="s">
         <v>66</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C54" s="5" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C54" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D54" s="6" t="s">
+      <c r="D54" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="C55" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" s="6" t="s">
+    <row r="55" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C55" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C56" s="5" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C56" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="10"/>
-      <c r="B57" s="11"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="5"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="7"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
         <v>13</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C58" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D58" s="6" t="s">
+      <c r="D58" s="4" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C59" s="5" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C59" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="D59" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="C60" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D60" s="6" t="s">
+    <row r="60" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C60" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C61" s="5" t="s">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C61" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="D61" s="4" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="10"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="12"/>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="4">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="5"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="7"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
         <v>14</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C63" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D63" s="6" t="s">
+      <c r="D63" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C64" s="5" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C64" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D64" s="6" t="s">
+      <c r="D64" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C65" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D65" s="6" t="s">
+    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C65" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="5" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C66" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D66" s="6" t="s">
+      <c r="D66" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="67" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="10"/>
-      <c r="B67" s="11"/>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="2"/>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="5"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
         <v>15</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C68" s="5" t="s">
+      <c r="C68" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D68" s="6" t="s">
+      <c r="D68" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C69" s="5" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C69" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D69" s="6" t="s">
+      <c r="D69" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="C70" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D70" s="6" t="s">
+    <row r="70" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C70" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C71" s="5" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C71" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="10"/>
-      <c r="B72" s="11"/>
-      <c r="C72" s="12"/>
-      <c r="D72" s="12"/>
-      <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
-      <c r="G72" s="2"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="5"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
         <v>16</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C73" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D73" s="6" t="s">
+      <c r="D73" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C74" s="5" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C74" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D74" s="6" t="s">
+      <c r="D74" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="C75" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D75" s="6" t="s">
+    <row r="75" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="C75" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C76" s="5" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C76" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="10"/>
-      <c r="B77" s="11"/>
-      <c r="C77" s="12"/>
-      <c r="D77" s="12"/>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2"/>
-      <c r="G77" s="2"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="5"/>
+      <c r="B77" s="6"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
         <v>17</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C78" s="5" t="s">
+      <c r="C78" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D78" s="6" t="s">
+      <c r="D78" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C79" s="5" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C79" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D79" s="6" t="s">
+      <c r="D79" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="C80" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D80" s="6" t="s">
+    <row r="80" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="C80" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D80" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C81" s="5" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C81" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="10"/>
-      <c r="B82" s="11"/>
-      <c r="C82" s="12"/>
-      <c r="D82" s="12"/>
-      <c r="E82" s="2"/>
-      <c r="F82" s="2"/>
-      <c r="G82" s="2"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="5"/>
+      <c r="B82" s="6"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="7"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
         <v>18</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B83" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C83" s="5" t="s">
+      <c r="C83" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D83" s="6" t="s">
+      <c r="D83" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C84" s="5" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C84" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D84" s="6" t="s">
+      <c r="D84" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="C85" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D85" s="6" t="s">
+    <row r="85" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C85" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D85" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C86" s="5" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C86" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="10"/>
-      <c r="B87" s="11"/>
-      <c r="C87" s="12"/>
-      <c r="D87" s="12"/>
-      <c r="E87" s="2"/>
-      <c r="F87" s="2"/>
-      <c r="G87" s="2"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="5"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
         <v>19</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C88" s="5" t="s">
+      <c r="C88" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D88" s="6" t="s">
+      <c r="D88" s="4" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C89" s="5" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C89" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D89" s="6" t="s">
+      <c r="D89" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="C90" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D90" s="6" t="s">
+    <row r="90" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C90" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D90" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C91" s="5" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C91" s="3" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="8"/>
+      <c r="B92" s="9"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="10"/>
+    </row>
+    <row r="93" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B93" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C93" s="13"/>
+      <c r="D93" s="13"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B94" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C94" s="13"/>
+      <c r="D94" s="13"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B95" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C95" s="13"/>
+      <c r="D95" s="13"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B96" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="C96" s="13"/>
+      <c r="D96" s="13"/>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B97" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C97" s="11"/>
+      <c r="D97" s="11"/>
+    </row>
+    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B98" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C98" s="11"/>
+      <c r="D98" s="11"/>
+    </row>
+    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B99" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C99" s="11"/>
+      <c r="D99" s="11"/>
+    </row>
+    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B100" s="11"/>
+      <c r="C100" s="11"/>
+      <c r="D100" s="11"/>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B101" s="12"/>
+      <c r="C101" s="12"/>
+      <c r="D101" s="12"/>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B102" s="12"/>
+      <c r="C102" s="12"/>
+      <c r="D102" s="12"/>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B103" s="12"/>
+      <c r="C103" s="12"/>
+      <c r="D103" s="12"/>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B104" s="12"/>
+      <c r="C104" s="12"/>
+      <c r="D104" s="12"/>
+    </row>
+    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B105" s="12"/>
+      <c r="C105" s="12"/>
+      <c r="D105" s="12"/>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B106" s="12"/>
+      <c r="C106" s="12"/>
+      <c r="D106" s="12"/>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B107" s="12"/>
+      <c r="C107" s="12"/>
+      <c r="D107" s="12"/>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B108" s="12"/>
+      <c r="C108" s="12"/>
+      <c r="D108" s="12"/>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B109" s="12"/>
+      <c r="C109" s="12"/>
+      <c r="D109" s="12"/>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B110" s="12"/>
+      <c r="C110" s="12"/>
+      <c r="D110" s="12"/>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B111" s="12"/>
+      <c r="C111" s="12"/>
+      <c r="D111" s="12"/>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B112" s="12"/>
+      <c r="C112" s="12"/>
+      <c r="D112" s="12"/>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B113" s="12"/>
+      <c r="C113" s="12"/>
+      <c r="D113" s="12"/>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B114" s="12"/>
+      <c r="C114" s="12"/>
+      <c r="D114" s="12"/>
+    </row>
+    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B115" s="12"/>
+      <c r="C115" s="12"/>
+      <c r="D115" s="12"/>
+    </row>
+    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B116" s="12"/>
+      <c r="C116" s="12"/>
+      <c r="D116" s="12"/>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B117" s="12"/>
+      <c r="C117" s="12"/>
+      <c r="D117" s="12"/>
+    </row>
+    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="12"/>
+      <c r="C118" s="12"/>
+      <c r="D118" s="12"/>
+    </row>
+    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B119" s="12"/>
+      <c r="C119" s="12"/>
+      <c r="D119" s="12"/>
+    </row>
+    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="12"/>
+      <c r="C120" s="12"/>
+      <c r="D120" s="12"/>
+    </row>
+    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="12"/>
+      <c r="C121" s="12"/>
+      <c r="D121" s="12"/>
+    </row>
+    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B122" s="12"/>
+      <c r="C122" s="12"/>
+      <c r="D122" s="12"/>
+    </row>
+    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B123" s="12"/>
+      <c r="C123" s="12"/>
+      <c r="D123" s="12"/>
+    </row>
+    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B124" s="12"/>
+      <c r="C124" s="12"/>
+      <c r="D124" s="12"/>
+    </row>
+    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="12"/>
+      <c r="C125" s="12"/>
+      <c r="D125" s="12"/>
+    </row>
+    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B126" s="12"/>
+      <c r="C126" s="12"/>
+      <c r="D126" s="12"/>
+    </row>
+    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B127" s="12"/>
+      <c r="C127" s="12"/>
+      <c r="D127" s="12"/>
+    </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B99:D100"/>
+    <mergeCell ref="B93:D93"/>
+    <mergeCell ref="B94:D94"/>
+    <mergeCell ref="B95:D95"/>
+    <mergeCell ref="B96:D96"/>
+    <mergeCell ref="B97:D97"/>
+    <mergeCell ref="B98:D98"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>